<commit_message>
Funcao Desloc - Retornar Coluna e Uso na Validacao de Dados
</commit_message>
<xml_diff>
--- a/5-FuncoesMercadoTrabalho/61. Função DESLOC - Retornar Coluna - Material(1).xlsx
+++ b/5-FuncoesMercadoTrabalho/61. Função DESLOC - Retornar Coluna - Material(1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 8 - Funções Mercado de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\5-FuncoesMercadoTrabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F0D948-074E-4506-89CF-CF9A58B366C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D29102-7413-4149-A55A-B7A162209C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C3784EBB-09BF-477B-9CB0-C14E8EE5D46B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C3784EBB-09BF-477B-9CB0-C14E8EE5D46B}"/>
   </bookViews>
   <sheets>
     <sheet name="DESLOC1" sheetId="4" r:id="rId1"/>
@@ -34,6 +34,9 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -302,7 +305,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -379,23 +382,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -420,9 +413,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -460,7 +453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -566,7 +559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -708,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -718,15 +711,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B1136E-754E-4280-901A-BBABC8B877E8}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="10.6640625" customWidth="1"/>
-    <col min="9" max="10" width="12.33203125" customWidth="1"/>
+    <col min="1" max="7" width="10.7109375" customWidth="1"/>
+    <col min="9" max="10" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -755,7 +748,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -784,7 +777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -809,7 +802,7 @@
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -839,7 +832,7 @@
         <v>4759</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -862,7 +855,7 @@
         <v>4640</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -885,7 +878,7 @@
         <v>5492</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -908,7 +901,7 @@
         <v>7819</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -931,7 +924,7 @@
         <v>8236</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -954,7 +947,7 @@
         <v>9554</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -977,7 +970,7 @@
         <v>5129</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
@@ -1000,7 +993,7 @@
         <v>3647</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -1023,7 +1016,7 @@
         <v>4328</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
@@ -1046,7 +1039,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -1069,7 +1062,7 @@
         <v>8413</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1092,7 +1085,7 @@
         <v>9957</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1108,7 @@
         <v>6982</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
@@ -1138,7 +1131,7 @@
         <v>5958</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
@@ -1161,7 +1154,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -1184,7 +1177,7 @@
         <v>8359</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1200,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
@@ -1232,10 +1225,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:G21">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>$J$4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$J$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1253,19 +1243,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898E6AFE-48E2-4D7F-A388-E1EF0FB9FA17}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="7" width="10.6640625" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.28515625" customWidth="1"/>
     <col min="11" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1288,7 +1278,7 @@
         <v>43983</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1318,7 +1308,7 @@
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1349,7 +1339,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1372,7 +1362,7 @@
         <v>2812</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1401,7 +1391,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -1431,7 +1421,7 @@
         <v>27785</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -1454,7 +1444,7 @@
         <v>7819</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +1467,7 @@
         <v>8236</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -1500,7 +1490,7 @@
         <v>9554</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -1523,7 +1513,7 @@
         <v>5129</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
@@ -1546,7 +1536,7 @@
         <v>3647</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -1569,7 +1559,7 @@
         <v>4328</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
@@ -1592,7 +1582,7 @@
         <v>2892</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -1615,7 +1605,7 @@
         <v>8413</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -1638,7 +1628,7 @@
         <v>9957</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -1661,7 +1651,7 @@
         <v>6982</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
@@ -1684,7 +1674,7 @@
         <v>5958</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
@@ -1707,7 +1697,7 @@
         <v>3850</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -1730,7 +1720,7 @@
         <v>8359</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>21</v>
       </c>
@@ -1753,7 +1743,7 @@
         <v>5767</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
@@ -1776,7 +1766,7 @@
         <v>8837</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1801,20 +1791,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76432A4A-E783-42D8-A1BF-7DE4A5EEBAAF}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="7" width="10.6640625" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="7" width="10.7109375" style="2" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="11" width="11.44140625" customWidth="1"/>
+    <col min="10" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>2</v>
       </c>
@@ -1843,7 +1835,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -1869,12 +1861,12 @@
         <v>3</v>
       </c>
       <c r="J2" s="13" cm="1">
-        <f t="array" aca="1" ref="J2:J21" ca="1">OFFSET(A2,0,MATCH(J1,B1:G1,0),20,1)</f>
+        <f t="array" aca="1" ref="J2:J21" ca="1">OFFSET(A2:A21,0,MATCH(J1,B1:G1,0), 20)</f>
         <v>7459</v>
       </c>
       <c r="K2" s="13"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1905,7 +1897,7 @@
       </c>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1936,7 +1928,7 @@
       </c>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -1967,7 +1959,7 @@
       </c>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +1990,7 @@
       </c>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2029,7 +2021,7 @@
       </c>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -2060,7 +2052,7 @@
       </c>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
@@ -2091,7 +2083,7 @@
       </c>
       <c r="K9" s="13"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2122,7 +2114,7 @@
       </c>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>12</v>
       </c>
@@ -2153,7 +2145,7 @@
       </c>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -2184,7 +2176,7 @@
       </c>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
@@ -2215,7 +2207,7 @@
       </c>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -2246,7 +2238,7 @@
       </c>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -2277,7 +2269,7 @@
       </c>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>17</v>
       </c>
@@ -2308,7 +2300,7 @@
       </c>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>18</v>
       </c>
@@ -2339,7 +2331,7 @@
       </c>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
@@ -2370,7 +2362,7 @@
       </c>
       <c r="K18" s="13"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -2401,7 +2393,7 @@
       </c>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>21</v>
       </c>
@@ -2432,7 +2424,7 @@
       </c>
       <c r="K20" s="13"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>22</v>
       </c>
@@ -2463,7 +2455,7 @@
       </c>
       <c r="K21" s="13"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2486,17 +2478,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B31B1128-45F1-419F-A495-5046DFEF50D3}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="4" max="5" width="20.21875" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="4" max="5" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -2504,16 +2498,16 @@
         <v>23</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2521,14 +2515,14 @@
         <v>30</v>
       </c>
       <c r="D2" t="str" cm="1">
-        <f t="array" aca="1" ref="D2:D8" ca="1">OFFSET(A1,MATCH(D1,A2:A27,0),1,COUNTIFS(A:A,D1),1)</f>
-        <v>Pará</v>
+        <f t="array" aca="1" ref="D2:D10" ca="1">OFFSET(A1,MATCH(D1,A2:A27,0),1,COUNTIFS(A1:A27,D1))</f>
+        <v>Bahia</v>
       </c>
       <c r="J2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2537,13 +2531,13 @@
       </c>
       <c r="D3" t="str">
         <f ca="1"/>
-        <v>Tocantins</v>
+        <v>Piauí</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2552,13 +2546,13 @@
       </c>
       <c r="D4" t="str">
         <f ca="1"/>
-        <v>Amazonas</v>
+        <v>Paraíba</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -2567,13 +2561,13 @@
       </c>
       <c r="D5" t="str">
         <f ca="1"/>
-        <v>Rondônia</v>
+        <v>Maranhão</v>
       </c>
       <c r="J5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2582,10 +2576,10 @@
       </c>
       <c r="D6" t="str">
         <f ca="1"/>
-        <v>Acre</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Pernambuco</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2594,10 +2588,10 @@
       </c>
       <c r="D7" t="str">
         <f ca="1"/>
-        <v>Amapá</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Ceará</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2606,26 +2600,34 @@
       </c>
       <c r="D8" t="str">
         <f ca="1"/>
-        <v>Roraima</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>Rio Grande do Norte</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D9" t="str">
+        <f ca="1"/>
+        <v>Alagoas</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D10" t="str">
+        <f ca="1"/>
+        <v>Sergipe</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2641,7 +2643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2649,7 +2651,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2657,7 +2659,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2665,7 +2667,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2673,7 +2675,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2689,7 +2691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2697,7 +2699,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2705,7 +2707,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2713,7 +2715,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2721,7 +2723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2729,7 +2731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2737,7 +2739,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -2745,7 +2747,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2755,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2762,12 +2764,15 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{9A08786D-1F8E-4086-AE35-22F2B4820A34}">
       <formula1>$J$1:$J$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{4FFD6F3D-73C4-4B68-B08A-681EDDA25116}">
-      <formula1>OFFSET(A1,MATCH(D1,A2:A27,0),1,COUNTIFS(A:A,D1),1)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{F857C183-2217-43FA-B68A-4365298B0F28}">
+      <formula1>OFFSET(A1,MATCH(D1,A2:A27,0),1,COUNTIFS(A1:A27,D1))</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{9C54703D-EFE2-4467-8C56-8F7EB2B72EB6}">
+      <formula1>OFFSET(A1,MATCH(D1,A2:A27,0),1,COUNTIFS(A1:A27,D1))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>